<commit_message>
adding comment to tab
</commit_message>
<xml_diff>
--- a/docs/graviton_rev1_netlist.xlsx
+++ b/docs/graviton_rev1_netlist.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16875"/>
   </bookViews>
   <sheets>
-    <sheet name="graviton_rev1_netlist" sheetId="1" r:id="rId1"/>
+    <sheet name="U14(CONFIG)" sheetId="1" r:id="rId1"/>
     <sheet name="U19A(ETH)" sheetId="2" r:id="rId2"/>
     <sheet name="U19B(ADC)" sheetId="3" r:id="rId3"/>
     <sheet name="U19C(DAC)" sheetId="4" r:id="rId4"/>
@@ -5906,8 +5906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>